<commit_message>
Estimación boot smce empleo y educación -SG
</commit_message>
<xml_diff>
--- a/Frecuentista_depto/COL/Output/educacion_smce_MC.xlsx
+++ b/Frecuentista_depto/COL/Output/educacion_smce_MC.xlsx
@@ -467,10 +467,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0025179940681135</v>
+        <v>0.00236655069326775</v>
       </c>
       <c r="C2" t="n">
-        <v>0.655178147337734</v>
+        <v>0.649198730991558</v>
       </c>
     </row>
     <row r="3">
@@ -478,10 +478,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>0.00294347151255848</v>
+        <v>0.00273222834405392</v>
       </c>
       <c r="C3" t="n">
-        <v>0.545760792802278</v>
+        <v>0.542272216357288</v>
       </c>
     </row>
     <row r="4">
@@ -489,10 +489,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>0.00331013924869937</v>
+        <v>0.00279248261528358</v>
       </c>
       <c r="C4" t="n">
-        <v>0.584257248244939</v>
+        <v>0.58431274528565</v>
       </c>
     </row>
     <row r="5">
@@ -500,10 +500,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.00329464002643162</v>
+        <v>0.00281627144216852</v>
       </c>
       <c r="C5" t="n">
-        <v>0.660202422564358</v>
+        <v>0.647318447403382</v>
       </c>
     </row>
     <row r="6">
@@ -511,10 +511,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>0.00301425248825789</v>
+        <v>0.00318674057032065</v>
       </c>
       <c r="C6" t="n">
-        <v>0.706406892158707</v>
+        <v>0.699363159911048</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +522,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>0.00322219704967708</v>
+        <v>0.00334827073445093</v>
       </c>
       <c r="C7" t="n">
-        <v>0.629263253306681</v>
+        <v>0.623141254306129</v>
       </c>
     </row>
     <row r="8">
@@ -533,10 +533,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>0.00322447454699984</v>
+        <v>0.00321848395386037</v>
       </c>
       <c r="C8" t="n">
-        <v>0.759273387864691</v>
+        <v>0.746260244142302</v>
       </c>
     </row>
     <row r="9">
@@ -544,10 +544,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>0.00314225889490209</v>
+        <v>0.00264247241616706</v>
       </c>
       <c r="C9" t="n">
-        <v>0.754258476025202</v>
+        <v>0.739854415825333</v>
       </c>
     </row>
     <row r="10">
@@ -555,10 +555,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>0.00318853097715189</v>
+        <v>0.00289923695065701</v>
       </c>
       <c r="C10" t="n">
-        <v>0.658954309414708</v>
+        <v>0.649918885562665</v>
       </c>
     </row>
     <row r="11">
@@ -566,10 +566,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>0.00357330417328073</v>
+        <v>0.0027343908310323</v>
       </c>
       <c r="C11" t="n">
-        <v>0.667864450409708</v>
+        <v>0.643772520705782</v>
       </c>
     </row>
     <row r="12">
@@ -577,10 +577,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>0.00606580543977915</v>
+        <v>0.00543972911234428</v>
       </c>
       <c r="C12" t="n">
-        <v>0.622873672257652</v>
+        <v>0.62065986148731</v>
       </c>
     </row>
     <row r="13">
@@ -588,10 +588,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>0.00723095701946919</v>
+        <v>0.00309196118596838</v>
       </c>
       <c r="C13" t="n">
-        <v>0.81532268512828</v>
+        <v>0.766862976337199</v>
       </c>
     </row>
     <row r="14">
@@ -599,10 +599,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="n">
-        <v>0.00290309932812651</v>
+        <v>0.00305906564565818</v>
       </c>
       <c r="C14" t="n">
-        <v>0.685419467310296</v>
+        <v>0.682143343498224</v>
       </c>
     </row>
     <row r="15">
@@ -610,10 +610,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>0.00448590551640666</v>
+        <v>0.00281137806399219</v>
       </c>
       <c r="C15" t="n">
-        <v>0.797210877658834</v>
+        <v>0.780488510496068</v>
       </c>
     </row>
     <row r="16">
@@ -621,10 +621,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="n">
-        <v>0.00288508582898144</v>
+        <v>0.00267788758712278</v>
       </c>
       <c r="C16" t="n">
-        <v>0.622967626558145</v>
+        <v>0.609383735684052</v>
       </c>
     </row>
     <row r="17">
@@ -632,10 +632,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>0.00298862907653914</v>
+        <v>0.00333296035881704</v>
       </c>
       <c r="C17" t="n">
-        <v>0.620593559195776</v>
+        <v>0.613977858195642</v>
       </c>
     </row>
     <row r="18">
@@ -643,10 +643,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0037742043615148</v>
+        <v>0.00259529550156573</v>
       </c>
       <c r="C18" t="n">
-        <v>0.728163532046818</v>
+        <v>0.711548390955164</v>
       </c>
     </row>
     <row r="19">
@@ -654,10 +654,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>0.00322076559321273</v>
+        <v>0.00283870272538234</v>
       </c>
       <c r="C19" t="n">
-        <v>0.658249646143652</v>
+        <v>0.650055774033806</v>
       </c>
     </row>
     <row r="20">
@@ -665,10 +665,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="n">
-        <v>0.00312838585096793</v>
+        <v>0.00334363662860974</v>
       </c>
       <c r="C20" t="n">
-        <v>0.599527855860495</v>
+        <v>0.597313954514135</v>
       </c>
     </row>
     <row r="21">
@@ -676,10 +676,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="n">
-        <v>0.00342175744658777</v>
+        <v>0.00348133952728797</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6366670305999</v>
+        <v>0.634096255422113</v>
       </c>
     </row>
     <row r="22">
@@ -687,10 +687,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="n">
-        <v>0.00307391621227903</v>
+        <v>0.00299047492118853</v>
       </c>
       <c r="C22" t="n">
-        <v>0.616639910703086</v>
+        <v>0.607996562858367</v>
       </c>
     </row>
     <row r="23">
@@ -698,10 +698,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="n">
-        <v>0.0029842063200593</v>
+        <v>0.00289508774243836</v>
       </c>
       <c r="C23" t="n">
-        <v>0.733247614291178</v>
+        <v>0.717438195996371</v>
       </c>
     </row>
     <row r="24">
@@ -709,10 +709,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="n">
-        <v>0.00293384286184778</v>
+        <v>0.00306790351104019</v>
       </c>
       <c r="C24" t="n">
-        <v>0.646309169899082</v>
+        <v>0.639330681291519</v>
       </c>
     </row>
     <row r="25">
@@ -720,10 +720,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="n">
-        <v>0.00250258627582739</v>
+        <v>0.00266115520863512</v>
       </c>
       <c r="C25" t="n">
-        <v>0.549128624164246</v>
+        <v>0.545079597601623</v>
       </c>
     </row>
     <row r="26">
@@ -731,10 +731,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="n">
-        <v>0.0293218269551992</v>
+        <v>0.030933790595386</v>
       </c>
       <c r="C26" t="n">
-        <v>0.737879475586125</v>
+        <v>0.716618950357581</v>
       </c>
     </row>
     <row r="27">
@@ -742,10 +742,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="n">
-        <v>0.0314327836848372</v>
+        <v>0.0328945591194969</v>
       </c>
       <c r="C27" t="n">
-        <v>0.685955370946278</v>
+        <v>0.674813101041297</v>
       </c>
     </row>
     <row r="28">
@@ -753,10 +753,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="n">
-        <v>0.0251585494580435</v>
+        <v>0.0281971644818462</v>
       </c>
       <c r="C28" t="n">
-        <v>0.750916659813165</v>
+        <v>0.728783640612074</v>
       </c>
     </row>
     <row r="29">
@@ -764,10 +764,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="n">
-        <v>0.0528782857201459</v>
+        <v>0.0535874616100596</v>
       </c>
       <c r="C29" t="n">
-        <v>0.600285563612393</v>
+        <v>0.581046802900461</v>
       </c>
     </row>
     <row r="30">
@@ -775,10 +775,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="n">
-        <v>0.0244932265124807</v>
+        <v>0.0334513327190158</v>
       </c>
       <c r="C30" t="n">
-        <v>0.782568478718921</v>
+        <v>0.75391440745423</v>
       </c>
     </row>
     <row r="31">
@@ -786,10 +786,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="n">
-        <v>0.0221135875406694</v>
+        <v>0.025156712332445</v>
       </c>
       <c r="C31" t="n">
-        <v>0.805449763086222</v>
+        <v>0.778394955788531</v>
       </c>
     </row>
     <row r="32">
@@ -797,10 +797,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0267625024128747</v>
+        <v>0.0303442538926168</v>
       </c>
       <c r="C32" t="n">
-        <v>0.749277438907431</v>
+        <v>0.727860705106073</v>
       </c>
     </row>
     <row r="33">
@@ -808,10 +808,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0208853158436309</v>
+        <v>0.0260115006088414</v>
       </c>
       <c r="C33" t="n">
-        <v>0.837465418072919</v>
+        <v>0.806954413652137</v>
       </c>
     </row>
     <row r="34">
@@ -819,10 +819,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0215684667107427</v>
+        <v>0.022669706968705</v>
       </c>
       <c r="C34" t="n">
-        <v>0.824413163401179</v>
+        <v>0.79637964195887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>